<commit_message>
docs: review doc and cols in hkdistrict_summary
</commit_message>
<xml_diff>
--- a/.dev/data/hkdistrictsummary.xlsx
+++ b/.dev/data/hkdistrictsummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Chan\Documents\SourceTree Repos\hkdatasets\.dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2C61D-15FB-4D8E-B559-CAF0C7CB69DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146ED060-718A-4072-B027-7DF0F6050E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="45" windowWidth="28800" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>Code</t>
   </si>
@@ -254,6 +254,21 @@
   </si>
   <si>
     <t>Is</t>
+  </si>
+  <si>
+    <t>Region_EN</t>
+  </si>
+  <si>
+    <t>Hong Kong Island</t>
+  </si>
+  <si>
+    <t>Kowloon</t>
+  </si>
+  <si>
+    <t>New Territories West</t>
+  </si>
+  <si>
+    <t>New Territories East</t>
   </si>
 </sst>
 </file>
@@ -640,20 +655,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,13 +680,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -681,13 +700,16 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -698,13 +720,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -715,13 +740,16 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -732,13 +760,16 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -749,13 +780,16 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -766,13 +800,16 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -783,13 +820,16 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -800,13 +840,16 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -817,13 +860,16 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -834,13 +880,16 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -851,13 +900,16 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -868,13 +920,16 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -885,13 +940,16 @@
         <v>45</v>
       </c>
       <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -902,13 +960,16 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -919,13 +980,16 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -936,13 +1000,16 @@
         <v>55</v>
       </c>
       <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -953,13 +1020,16 @@
         <v>58</v>
       </c>
       <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -970,9 +1040,12 @@
         <v>61</v>
       </c>
       <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>